<commit_message>
Finished adding question methods
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="138">
   <si>
     <t>Entity</t>
   </si>
@@ -427,13 +427,16 @@
   </si>
   <si>
     <t>http://api.stackexchange.com/docs/types/related-site</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,13 +452,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -467,16 +482,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -779,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +896,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1024,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,31 +1078,49 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1135,21 +1171,33 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -1170,46 +1218,73 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B36" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Added Revision, Search, and Similiar methods
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
   <si>
     <t>Entity</t>
   </si>
@@ -1042,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,6 +1295,9 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Worked on Tag, Stats, and user methods.
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="140">
   <si>
     <t>Entity</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>TagScore</t>
+  </si>
+  <si>
+    <t>http://api.stackexchange.com/docs/types/tag-score</t>
   </si>
 </sst>
 </file>
@@ -795,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +910,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -936,7 +942,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1005,6 +1011,14 @@
       </c>
       <c r="C25" s="1" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1033,8 +1047,10 @@
     <hyperlink ref="C2" r:id="rId22"/>
     <hyperlink ref="C25" r:id="rId23"/>
     <hyperlink ref="C24" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -1042,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,11 +1324,17 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B40" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B41" t="s">
         <v>43</v>
       </c>
@@ -1323,11 +1345,17 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B43" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B44" t="s">
         <v>45</v>
       </c>
@@ -1338,6 +1366,9 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B46" t="s">
         <v>48</v>
       </c>
@@ -1348,31 +1379,49 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B48" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B49" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B51" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B52" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B53" t="s">
         <v>55</v>
       </c>
@@ -1383,31 +1432,49 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B55" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B56" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B57" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B58" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B59" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B60" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Added more user methods
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="140">
   <si>
     <t>Entity</t>
   </si>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,51 +1480,81 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B61" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B62" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B63" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B64" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B65" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B66" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B67" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B68" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B69" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B70" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Added network methods and finished user methods
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="140">
   <si>
     <t>Entity</t>
   </si>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,36 +1560,57 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B71" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B72" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B73" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B74" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B75" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B76" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B77" t="s">
         <v>80</v>
       </c>
@@ -1609,42 +1630,54 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B81" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B82" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B83" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B84" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Started adding async methods
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="145">
   <si>
     <t>Entity</t>
   </si>
@@ -436,6 +436,21 @@
   </si>
   <si>
     <t>http://api.stackexchange.com/docs/types/tag-score</t>
+  </si>
+  <si>
+    <t>Synchronus</t>
+  </si>
+  <si>
+    <t>Asynchronus</t>
+  </si>
+  <si>
+    <t>.Net 3.5</t>
+  </si>
+  <si>
+    <t>Integration Test</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -1056,112 +1071,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -1630,54 +1737,81 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B81" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>137</v>
+      </c>
+      <c r="D81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B82" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>137</v>
+      </c>
+      <c r="D82" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B83" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>137</v>
+      </c>
+      <c r="D83" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B84" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>137</v>
+      </c>
+      <c r="D84" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="B88" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Finished porting all implemented methods to async
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="145">
   <si>
     <t>Entity</t>
   </si>
@@ -1073,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,164 +1273,254 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B36" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>137</v>
       </c>
@@ -1438,7 +1528,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>137</v>
       </c>
@@ -1446,293 +1536,497 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B46" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D48" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B49" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B50" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B51" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B52" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B53" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B55" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>137</v>
+      </c>
+      <c r="D55" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B56" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B57" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B58" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B59" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B60" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>137</v>
+      </c>
+      <c r="D60" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B61" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B62" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>137</v>
+      </c>
+      <c r="D62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B63" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D63" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B64" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>137</v>
+      </c>
+      <c r="D64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B65" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>137</v>
+      </c>
+      <c r="D65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B66" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B67" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B68" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B69" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B70" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>137</v>
+      </c>
+      <c r="D70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B71" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B72" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B73" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B74" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>137</v>
+      </c>
+      <c r="D74" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B75" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>137</v>
+      </c>
+      <c r="D75" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B76" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B77" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>137</v>
+      </c>
+      <c r="D77" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>137</v>
+      </c>
+      <c r="D78" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>137</v>
+      </c>
+      <c r="D79" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -1814,6 +2108,12 @@
       </c>
       <c r="B88" t="s">
         <v>83</v>
+      </c>
+      <c r="C88" t="s">
+        <v>137</v>
+      </c>
+      <c r="D88" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a UnixDateTime class. I may not end up keeping it.
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="145">
   <si>
     <t>Entity</t>
   </si>
@@ -1073,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,6 +1121,9 @@
       <c r="D2" t="s">
         <v>137</v>
       </c>
+      <c r="E2" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1133,6 +1136,9 @@
         <v>137</v>
       </c>
       <c r="D3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1144,6 +1150,9 @@
         <v>137</v>
       </c>
       <c r="D4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more 3.5 client methods
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="146">
   <si>
     <t>Entity</t>
   </si>
@@ -451,6 +451,9 @@
   </si>
   <si>
     <t>Documentation</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -1073,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,6 +1177,9 @@
       <c r="D6" t="s">
         <v>137</v>
       </c>
+      <c r="E6" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1188,6 +1194,9 @@
       <c r="D7" t="s">
         <v>137</v>
       </c>
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1202,6 +1211,9 @@
       <c r="D8" t="s">
         <v>137</v>
       </c>
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1216,6 +1228,9 @@
       <c r="D9" t="s">
         <v>137</v>
       </c>
+      <c r="E9" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1230,6 +1245,9 @@
       <c r="D10" t="s">
         <v>137</v>
       </c>
+      <c r="E10" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1242,6 +1260,9 @@
         <v>137</v>
       </c>
       <c r="D11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1260,6 +1281,9 @@
       <c r="D13" t="s">
         <v>137</v>
       </c>
+      <c r="E13" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1271,6 +1295,9 @@
       <c r="D14" t="s">
         <v>137</v>
       </c>
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1282,27 +1309,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>137</v>
       </c>
@@ -1315,8 +1342,11 @@
       <c r="D21" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>137</v>
       </c>
@@ -1329,8 +1359,11 @@
       <c r="D22" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>137</v>
       </c>
@@ -1343,8 +1376,11 @@
       <c r="D23" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>137</v>
       </c>
@@ -1357,13 +1393,16 @@
       <c r="D24" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>28</v>
       </c>
@@ -1373,13 +1412,16 @@
       <c r="D26" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>137</v>
       </c>
@@ -1392,8 +1434,11 @@
       <c r="D28" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>137</v>
       </c>
@@ -1406,8 +1451,11 @@
       <c r="D29" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>137</v>
       </c>
@@ -1420,8 +1468,11 @@
       <c r="D30" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>137</v>
       </c>
@@ -1434,8 +1485,11 @@
       <c r="D31" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>137</v>
       </c>
@@ -1448,8 +1502,11 @@
       <c r="D32" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>137</v>
       </c>
@@ -1462,8 +1519,11 @@
       <c r="D33" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -1476,8 +1536,11 @@
       <c r="D34" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>137</v>
       </c>
@@ -1490,8 +1553,11 @@
       <c r="D35" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>137</v>
       </c>
@@ -1504,13 +1570,16 @@
       <c r="D36" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>137</v>
       </c>
@@ -1523,13 +1592,16 @@
       <c r="D38" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>137</v>
       </c>
@@ -1537,7 +1609,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>137</v>
       </c>
@@ -1545,12 +1617,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>137</v>
       </c>
@@ -1563,8 +1635,11 @@
       <c r="D43" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>137</v>
       </c>
@@ -1577,13 +1652,16 @@
       <c r="D44" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>137</v>
       </c>
@@ -1596,13 +1674,16 @@
       <c r="D46" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>137</v>
       </c>
@@ -1615,8 +1696,11 @@
       <c r="D48" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>137</v>
       </c>
@@ -1629,8 +1713,11 @@
       <c r="D49" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>137</v>
       </c>
@@ -1643,8 +1730,11 @@
       <c r="D50" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>137</v>
       </c>
@@ -1657,8 +1747,11 @@
       <c r="D51" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>137</v>
       </c>
@@ -1671,8 +1764,11 @@
       <c r="D52" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>137</v>
       </c>
@@ -1685,13 +1781,16 @@
       <c r="D53" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>137</v>
       </c>
@@ -1704,8 +1803,11 @@
       <c r="D55" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>137</v>
       </c>
@@ -1718,8 +1820,11 @@
       <c r="D56" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>137</v>
       </c>
@@ -1732,8 +1837,11 @@
       <c r="D57" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>137</v>
       </c>
@@ -1746,8 +1854,11 @@
       <c r="D58" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>137</v>
       </c>
@@ -1760,8 +1871,11 @@
       <c r="D59" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>137</v>
       </c>
@@ -1774,8 +1888,11 @@
       <c r="D60" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>137</v>
       </c>
@@ -1788,8 +1905,11 @@
       <c r="D61" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>137</v>
       </c>
@@ -1802,8 +1922,11 @@
       <c r="D62" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>137</v>
       </c>
@@ -1816,8 +1939,11 @@
       <c r="D63" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>137</v>
       </c>
@@ -1830,8 +1956,11 @@
       <c r="D64" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>137</v>
       </c>
@@ -1844,8 +1973,11 @@
       <c r="D65" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>137</v>
       </c>
@@ -1858,8 +1990,11 @@
       <c r="D66" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>137</v>
       </c>
@@ -1872,8 +2007,11 @@
       <c r="D67" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>137</v>
       </c>
@@ -1886,8 +2024,11 @@
       <c r="D68" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>137</v>
       </c>
@@ -1900,8 +2041,11 @@
       <c r="D69" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>137</v>
       </c>
@@ -1914,8 +2058,11 @@
       <c r="D70" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>137</v>
       </c>
@@ -1928,8 +2075,11 @@
       <c r="D71" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>137</v>
       </c>
@@ -1942,8 +2092,11 @@
       <c r="D72" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>137</v>
       </c>
@@ -1956,8 +2109,11 @@
       <c r="D73" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>137</v>
       </c>
@@ -1970,8 +2126,11 @@
       <c r="D74" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>137</v>
       </c>
@@ -1984,8 +2143,11 @@
       <c r="D75" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>137</v>
       </c>
@@ -1998,8 +2160,11 @@
       <c r="D76" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>137</v>
       </c>
@@ -2012,8 +2177,11 @@
       <c r="D77" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>81</v>
       </c>
@@ -2023,8 +2191,11 @@
       <c r="D78" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>57</v>
       </c>
@@ -2034,8 +2205,11 @@
       <c r="D79" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
Almost done with the .net 3.5 async methods
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="147">
   <si>
     <t>Entity</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>.net 3.5 Async</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,11 +1090,12 @@
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1105,13 +1109,16 @@
         <v>142</v>
       </c>
       <c r="F1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" t="s">
         <v>143</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>137</v>
       </c>
@@ -1127,8 +1134,11 @@
       <c r="E2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>137</v>
       </c>
@@ -1144,8 +1154,11 @@
       <c r="E3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -1158,13 +1171,16 @@
       <c r="E4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>137</v>
       </c>
@@ -1180,8 +1196,11 @@
       <c r="E6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
@@ -1197,8 +1216,11 @@
       <c r="E7" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>137</v>
       </c>
@@ -1214,8 +1236,11 @@
       <c r="E8" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>137</v>
       </c>
@@ -1231,8 +1256,11 @@
       <c r="E9" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>137</v>
       </c>
@@ -1248,8 +1276,11 @@
       <c r="E10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>137</v>
       </c>
@@ -1265,13 +1296,16 @@
       <c r="E11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -1284,8 +1318,11 @@
       <c r="E13" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1298,38 +1335,41 @@
       <c r="E14" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>137</v>
       </c>
@@ -1345,8 +1385,11 @@
       <c r="E21" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>137</v>
       </c>
@@ -1362,8 +1405,11 @@
       <c r="E22" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>137</v>
       </c>
@@ -1379,8 +1425,11 @@
       <c r="E23" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>137</v>
       </c>
@@ -1396,13 +1445,16 @@
       <c r="E24" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>28</v>
       </c>
@@ -1416,12 +1468,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>137</v>
       </c>
@@ -1437,8 +1489,11 @@
       <c r="E28" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>137</v>
       </c>
@@ -1454,8 +1509,11 @@
       <c r="E29" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>137</v>
       </c>
@@ -1471,8 +1529,11 @@
       <c r="E30" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>137</v>
       </c>
@@ -1488,8 +1549,11 @@
       <c r="E31" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>137</v>
       </c>
@@ -1505,8 +1569,11 @@
       <c r="E32" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>137</v>
       </c>
@@ -1522,8 +1589,11 @@
       <c r="E33" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -1539,8 +1609,11 @@
       <c r="E34" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>137</v>
       </c>
@@ -1556,8 +1629,11 @@
       <c r="E35" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>137</v>
       </c>
@@ -1573,13 +1649,16 @@
       <c r="E36" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>137</v>
       </c>
@@ -1596,12 +1675,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>137</v>
       </c>
@@ -1609,7 +1688,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>137</v>
       </c>
@@ -1617,12 +1696,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>137</v>
       </c>
@@ -1639,7 +1718,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>137</v>
       </c>
@@ -1656,12 +1735,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>137</v>
       </c>
@@ -1678,12 +1757,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>137</v>
       </c>
@@ -1699,8 +1778,11 @@
       <c r="E48" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>137</v>
       </c>
@@ -1716,8 +1798,11 @@
       <c r="E49" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>137</v>
       </c>
@@ -1733,8 +1818,11 @@
       <c r="E50" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>137</v>
       </c>
@@ -1750,8 +1838,11 @@
       <c r="E51" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>137</v>
       </c>
@@ -1767,8 +1858,11 @@
       <c r="E52" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>137</v>
       </c>
@@ -1784,13 +1878,16 @@
       <c r="E53" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>137</v>
       </c>
@@ -1806,8 +1903,11 @@
       <c r="E55" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>137</v>
       </c>
@@ -1823,8 +1923,11 @@
       <c r="E56" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>137</v>
       </c>
@@ -1840,8 +1943,11 @@
       <c r="E57" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>137</v>
       </c>
@@ -1857,8 +1963,11 @@
       <c r="E58" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>137</v>
       </c>
@@ -1874,8 +1983,11 @@
       <c r="E59" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>137</v>
       </c>
@@ -1891,8 +2003,11 @@
       <c r="E60" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>137</v>
       </c>
@@ -1908,8 +2023,11 @@
       <c r="E61" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>137</v>
       </c>
@@ -1925,8 +2043,11 @@
       <c r="E62" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>137</v>
       </c>
@@ -1942,8 +2063,11 @@
       <c r="E63" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>137</v>
       </c>
@@ -1959,8 +2083,11 @@
       <c r="E64" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>137</v>
       </c>
@@ -1976,8 +2103,11 @@
       <c r="E65" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>137</v>
       </c>
@@ -1993,8 +2123,11 @@
       <c r="E66" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>137</v>
       </c>
@@ -2010,8 +2143,11 @@
       <c r="E67" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>137</v>
       </c>
@@ -2027,8 +2163,11 @@
       <c r="E68" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>137</v>
       </c>
@@ -2044,8 +2183,11 @@
       <c r="E69" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>137</v>
       </c>
@@ -2061,8 +2203,11 @@
       <c r="E70" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>137</v>
       </c>
@@ -2078,8 +2223,11 @@
       <c r="E71" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>137</v>
       </c>
@@ -2095,8 +2243,11 @@
       <c r="E72" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>137</v>
       </c>
@@ -2112,8 +2263,11 @@
       <c r="E73" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>137</v>
       </c>
@@ -2129,8 +2283,11 @@
       <c r="E74" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>137</v>
       </c>
@@ -2146,8 +2303,11 @@
       <c r="E75" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>137</v>
       </c>
@@ -2163,8 +2323,11 @@
       <c r="E76" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>137</v>
       </c>
@@ -2180,41 +2343,26 @@
       <c r="E77" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>81</v>
       </c>
-      <c r="C78" t="s">
-        <v>137</v>
-      </c>
-      <c r="D78" t="s">
-        <v>137</v>
-      </c>
-      <c r="E78" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>57</v>
       </c>
-      <c r="C79" t="s">
-        <v>137</v>
-      </c>
-      <c r="D79" t="s">
-        <v>137</v>
-      </c>
-      <c r="E79" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>137</v>
       </c>
@@ -2227,8 +2375,11 @@
       <c r="D81" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>137</v>
       </c>
@@ -2241,8 +2392,11 @@
       <c r="D82" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>137</v>
       </c>
@@ -2255,8 +2409,11 @@
       <c r="D83" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>137</v>
       </c>
@@ -2269,23 +2426,26 @@
       <c r="D84" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>137</v>
       </c>
@@ -2296,6 +2456,9 @@
         <v>137</v>
       </c>
       <c r="D88" t="s">
+        <v>137</v>
+      </c>
+      <c r="E88" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished the .net 3.5 async methods
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="147">
   <si>
     <t>Entity</t>
   </si>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,6 +1674,9 @@
       <c r="E38" t="s">
         <v>137</v>
       </c>
+      <c r="F38" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1717,6 +1720,9 @@
       <c r="E43" t="s">
         <v>137</v>
       </c>
+      <c r="F43" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
@@ -1732,6 +1738,9 @@
         <v>137</v>
       </c>
       <c r="E44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F44" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2362,7 +2371,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>137</v>
       </c>
@@ -2378,8 +2387,11 @@
       <c r="E81" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>137</v>
       </c>
@@ -2395,8 +2407,11 @@
       <c r="E82" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>137</v>
       </c>
@@ -2412,8 +2427,11 @@
       <c r="E83" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>137</v>
       </c>
@@ -2429,23 +2447,26 @@
       <c r="E84" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>137</v>
       </c>
@@ -2459,6 +2480,9 @@
         <v>137</v>
       </c>
       <c r="E88" t="s">
+        <v>137</v>
+      </c>
+      <c r="F88" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added support for apiKeys
</commit_message>
<xml_diff>
--- a/trunk/data/V2.0 Upgrade Checklist.xlsx
+++ b/trunk/data/V2.0 Upgrade Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="147">
   <si>
     <t>Entity</t>
   </si>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,6 +1363,18 @@
       <c r="B19" t="s">
         <v>21</v>
       </c>
+      <c r="C19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2455,10 +2467,34 @@
       <c r="B85" t="s">
         <v>88</v>
       </c>
+      <c r="C85" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" t="s">
+        <v>137</v>
+      </c>
+      <c r="E85" t="s">
+        <v>137</v>
+      </c>
+      <c r="F85" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>89</v>
+      </c>
+      <c r="C86" t="s">
+        <v>137</v>
+      </c>
+      <c r="D86" t="s">
+        <v>137</v>
+      </c>
+      <c r="E86" t="s">
+        <v>137</v>
+      </c>
+      <c r="F86" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>